<commit_message>
Preparation of test data and 246 - 258
</commit_message>
<xml_diff>
--- a/1st experiment backup/Obliczenia.xlsx
+++ b/1st experiment backup/Obliczenia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Documents\Wadaba\Eksperyment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01278A19-A08D-4359-85CC-220341B36221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8844E1-A200-4943-8BD9-CAD8162F8697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5CC8E75E-AE51-465C-ADEB-DC581107C77A}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{5CC8E75E-AE51-465C-ADEB-DC581107C77A}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>test</t>
   </si>
@@ -66,12 +66,21 @@
   </si>
   <si>
     <t>ile stopni obrotu</t>
+  </si>
+  <si>
+    <t>Moje poprawki</t>
+  </si>
+  <si>
+    <t>wyszło:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -135,6 +144,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B25697-28DF-4868-9050-AE4E2057114A}">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +479,7 @@
     <col min="8" max="8" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -487,7 +502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -517,7 +532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -538,8 +553,8 @@
         <f t="shared" ref="F4:F6" si="1">SUM(D4,E4)</f>
         <v>33000</v>
       </c>
-      <c r="G4" s="3">
-        <f t="shared" ref="G4:G6" si="2">F4/C4</f>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G5" si="2">F4/C4</f>
         <v>55</v>
       </c>
       <c r="H4" s="5">
@@ -547,7 +562,7 @@
         <v>6.5454545454545459</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -568,7 +583,7 @@
         <f t="shared" si="1"/>
         <v>33280</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="4">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
@@ -577,7 +592,7 @@
         <v>6.9230769230769234</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -598,14 +613,181 @@
         <f t="shared" si="1"/>
         <v>37440</v>
       </c>
-      <c r="G6" s="3">
-        <f t="shared" si="2"/>
+      <c r="G6" s="4">
+        <f>F6/C6</f>
         <v>72</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <f>C10/40</f>
+        <v>55</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2200</v>
+      </c>
+      <c r="D10" s="2">
+        <v>32400</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3600</v>
+      </c>
+      <c r="F10" s="7">
+        <f>SUM(D10,E10)</f>
+        <v>36000</v>
+      </c>
+      <c r="G10" s="4">
+        <f>F10/C10</f>
+        <v>16.363636363636363</v>
+      </c>
+      <c r="H10" s="2">
+        <f>360/G10</f>
+        <v>22</v>
+      </c>
+      <c r="J10">
+        <v>35200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ref="B11:B13" si="4">C11/40</f>
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>600</v>
+      </c>
+      <c r="D11" s="2">
+        <v>29700</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3300</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" ref="F11:F13" si="5">SUM(D11,E11)</f>
+        <v>33000</v>
+      </c>
+      <c r="G11" s="3">
+        <f>F11/C11</f>
+        <v>55</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" ref="H11:H13" si="6">360/G11</f>
+        <v>6.5454545454545459</v>
+      </c>
+      <c r="J11">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>640</v>
+      </c>
+      <c r="D12" s="2">
+        <v>29952</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3328</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="5"/>
+        <v>33280</v>
+      </c>
+      <c r="G12" s="4">
+        <f>F12/C12</f>
+        <v>52</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="6"/>
+        <v>6.9230769230769234</v>
+      </c>
+      <c r="J12" s="9">
+        <v>33280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="2">
+        <v>520</v>
+      </c>
+      <c r="D13" s="2">
+        <v>28080</v>
+      </c>
+      <c r="E13" s="2">
+        <f>D13*0.1</f>
+        <v>2808</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="5"/>
+        <v>30888</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F13/C13</f>
+        <v>59.4</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="6"/>
+        <v>6.0606060606060606</v>
+      </c>
+      <c r="J13">
+        <v>31200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>